<commit_message>
Arjun Committed Code on 10-30-2019
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="122">
   <si>
     <t>2IE</t>
   </si>
@@ -366,26 +366,41 @@
     <t>planCode,name,subscriptionId ,macInd</t>
   </si>
   <si>
-    <t>434349902</t>
-  </si>
-  <si>
-    <t>AugUser040</t>
-  </si>
-  <si>
     <t>id,status</t>
   </si>
   <si>
     <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/sub/v1/accounts/$BAN/subscriptions</t>
   </si>
   <si>
-    <t>ONREG-17965</t>
+    <t>ONREG-20535</t>
+  </si>
+  <si>
+    <t>ONREG-18520</t>
+  </si>
+  <si>
+    <t>ONREG-19643</t>
+  </si>
+  <si>
+    <t>ONREG-22679</t>
+  </si>
+  <si>
+    <t>ONREG-22710</t>
+  </si>
+  <si>
+    <t>ONREG-25767</t>
+  </si>
+  <si>
+    <t>ONREG-21172</t>
+  </si>
+  <si>
+    <t>ONREG-26222</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,8 +444,20 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,12 +477,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,13 +532,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -803,16 +824,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -823,21 +844,73 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>103562999</v>
-      </c>
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>107198053</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>124473304</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>169068211</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>113</v>
-      </c>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>225356050</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>244834015</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>114478789</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>172500199</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>205653581</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -880,13 +953,13 @@
         <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code Committed by arjun 10-31-2019
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="139">
   <si>
     <t>2IE</t>
   </si>
@@ -372,35 +372,86 @@
     <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/sub/v1/accounts/$BAN/subscriptions</t>
   </si>
   <si>
-    <t>ONREG-20535</t>
-  </si>
-  <si>
-    <t>ONREG-18520</t>
-  </si>
-  <si>
-    <t>ONREG-19643</t>
-  </si>
-  <si>
-    <t>ONREG-22679</t>
-  </si>
-  <si>
-    <t>ONREG-22710</t>
-  </si>
-  <si>
-    <t>ONREG-25767</t>
-  </si>
-  <si>
-    <t>ONREG-21172</t>
-  </si>
-  <si>
-    <t>ONREG-26222</t>
+    <t>ONREG-23902</t>
+  </si>
+  <si>
+    <t>ONREG-17938</t>
+  </si>
+  <si>
+    <t>ONREG-22294</t>
+  </si>
+  <si>
+    <t>ONREG-18131</t>
+  </si>
+  <si>
+    <t>ONREG-18240</t>
+  </si>
+  <si>
+    <t>ONREG-25876</t>
+  </si>
+  <si>
+    <t>ONREG-25888</t>
+  </si>
+  <si>
+    <t>ONREG-19423</t>
+  </si>
+  <si>
+    <t>ONREG-19642</t>
+  </si>
+  <si>
+    <t>ONREG-19769</t>
+  </si>
+  <si>
+    <t>ONREG-19795</t>
+  </si>
+  <si>
+    <t>ONREG-19814</t>
+  </si>
+  <si>
+    <t>ONREG-19836</t>
+  </si>
+  <si>
+    <t>ONREG-18965</t>
+  </si>
+  <si>
+    <t>ONREG-23937</t>
+  </si>
+  <si>
+    <t>ONREG-20446</t>
+  </si>
+  <si>
+    <t>ONREG-20191</t>
+  </si>
+  <si>
+    <t>ONREG-12902</t>
+  </si>
+  <si>
+    <t>ONREG-12961</t>
+  </si>
+  <si>
+    <t>ONREG-13268</t>
+  </si>
+  <si>
+    <t>ONREG-13351</t>
+  </si>
+  <si>
+    <t>ONREG-13415</t>
+  </si>
+  <si>
+    <t>ONREG-12927</t>
+  </si>
+  <si>
+    <t>ONREG-13024</t>
+  </si>
+  <si>
+    <t>ONREG-13036</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,18 +494,6 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -511,7 +550,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -532,15 +571,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
@@ -824,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,73 +876,213 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
-        <v>107198053</v>
-      </c>
-      <c r="B2" s="14" t="s">
+        <v>100147025</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <v>124473304</v>
-      </c>
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>101487374</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>169068211</v>
-      </c>
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>102440213</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>225356050</v>
-      </c>
-      <c r="B5" s="14" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>110062018</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>244834015</v>
-      </c>
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>127178114</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>114478789</v>
-      </c>
-      <c r="B7" s="14" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>139159854</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>172500199</v>
-      </c>
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>140389560</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <v>205653581</v>
-      </c>
-      <c r="B9" s="14" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>102440213</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>137199660</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10"/>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>100581355</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>135142501</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>102522400</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>109514216</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>119002359</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>108482050</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>163203979</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>146457800</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>119592056</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>164660957</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>113526468</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>150744017</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>131704213</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>131478014</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>139637466</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>142320256</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>124700667</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>138</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code committed by Arjun on 11-27-2019 Generic API data validation for account id API
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INPUT_SHEET" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="137">
   <si>
     <t>2IE</t>
   </si>
@@ -372,86 +372,80 @@
     <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/sub/v1/accounts/$BAN/subscriptions</t>
   </si>
   <si>
-    <t>ONREG-23902</t>
-  </si>
-  <si>
-    <t>ONREG-17938</t>
-  </si>
-  <si>
-    <t>ONREG-22294</t>
-  </si>
-  <si>
-    <t>ONREG-18131</t>
-  </si>
-  <si>
-    <t>ONREG-18240</t>
-  </si>
-  <si>
-    <t>ONREG-25876</t>
-  </si>
-  <si>
-    <t>ONREG-25888</t>
-  </si>
-  <si>
-    <t>ONREG-19423</t>
-  </si>
-  <si>
-    <t>ONREG-19642</t>
-  </si>
-  <si>
-    <t>ONREG-19769</t>
-  </si>
-  <si>
-    <t>ONREG-19795</t>
-  </si>
-  <si>
-    <t>ONREG-19814</t>
-  </si>
-  <si>
-    <t>ONREG-19836</t>
-  </si>
-  <si>
-    <t>ONREG-18965</t>
-  </si>
-  <si>
-    <t>ONREG-23937</t>
-  </si>
-  <si>
-    <t>ONREG-20446</t>
-  </si>
-  <si>
-    <t>ONREG-20191</t>
-  </si>
-  <si>
-    <t>ONREG-12902</t>
+    <t>434349902</t>
+  </si>
+  <si>
+    <t>AugUser040</t>
+  </si>
+  <si>
+    <t>4432447994</t>
+  </si>
+  <si>
+    <t>onreg-21213</t>
+  </si>
+  <si>
+    <t>ONREG-18091</t>
+  </si>
+  <si>
+    <t>ONREG-18095</t>
+  </si>
+  <si>
+    <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/accounts/v1/accounts/$BAN/financial-status?realTimeInd=false&amp;isGuestPay=false</t>
+  </si>
+  <si>
+    <t>financialstatus</t>
+  </si>
+  <si>
+    <t>ONREG-25212</t>
+  </si>
+  <si>
+    <t>ONREG-25329</t>
+  </si>
+  <si>
+    <t>ONREG-25213</t>
+  </si>
+  <si>
+    <t>ONREG-25783</t>
+  </si>
+  <si>
+    <t>future-payments</t>
+  </si>
+  <si>
+    <t>https://st1-apiservices-web.test.sprint.com:7441/api/process/pay/v1/accounts/$BAN/future-payments?realTimeInd=false&amp;isUsgBan=false</t>
+  </si>
+  <si>
+    <t>103341135</t>
+  </si>
+  <si>
+    <t>104404406</t>
+  </si>
+  <si>
+    <t>118789584</t>
+  </si>
+  <si>
+    <t>127188714</t>
+  </si>
+  <si>
+    <t>118919630</t>
+  </si>
+  <si>
+    <t>119134450</t>
   </si>
   <si>
     <t>ONREG-12961</t>
   </si>
   <si>
-    <t>ONREG-13268</t>
-  </si>
-  <si>
-    <t>ONREG-13351</t>
-  </si>
-  <si>
-    <t>ONREG-13415</t>
-  </si>
-  <si>
-    <t>ONREG-12927</t>
-  </si>
-  <si>
-    <t>ONREG-13024</t>
-  </si>
-  <si>
-    <t>ONREG-13036</t>
+    <t>https://st1-apiservices-web.test.sprint.com:7441/api/process/pay/v1/accounts/$BAN/payment-methods?isUsgBan=false&amp;isCheckAutoPayDiscount=true</t>
+  </si>
+  <si>
+    <t>payment-methods</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +488,13 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -550,7 +551,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -571,8 +572,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
@@ -856,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,211 +886,75 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
-        <v>100147025</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="12" t="s">
         <v>114</v>
       </c>
+      <c r="B2" s="14" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>101487374</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>115</v>
+      <c r="A3" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>102440213</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>116</v>
+      <c r="A4" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>110062018</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>117</v>
+      <c r="A5" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
-        <v>127178114</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>118</v>
+      <c r="A6" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
-        <v>139159854</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>119</v>
+      <c r="A7" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>140389560</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>120</v>
+      <c r="A8" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>102440213</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>116</v>
+      <c r="A9" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>137199660</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>100581355</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>135142501</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>102522400</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>109514216</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>119002359</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>108482050</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
-        <v>163203979</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>146457800</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
-        <v>119592056</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
-        <v>164660957</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+      <c r="A10" s="13">
         <v>113526468</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
-        <v>150744017</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
-        <v>131704213</v>
-      </c>
-      <c r="B23" s="12" t="s">
+      <c r="B10" s="15" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
-        <v>131478014</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
-        <v>139637466</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>142320256</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
-        <v>124700667</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1092,10 +965,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,7 +995,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>113</v>
@@ -1132,14 +1005,49 @@
       </c>
       <c r="D2" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Code is committed and upgraded to Maven project
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Eclipse\eclipse-workspace\eclipse-workspace\APIAutomaiton2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Eclipse\eclipse-workspace\eclipse-workspace\APIAutomaiton\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="INPUT_SHEET" sheetId="1" r:id="rId1"/>
@@ -867,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Code Committed by arjun on 12-04-2019 generic code 2 class created
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INPUT_SHEET" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId6"/>
     <sheet name="GUIDELINES" sheetId="3" r:id="rId7"/>
+    <sheet name="TestURLinfo" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="141">
   <si>
     <t>2IE</t>
   </si>
@@ -439,6 +440,18 @@
   </si>
   <si>
     <t>payment-methods</t>
+  </si>
+  <si>
+    <t>contracts</t>
+  </si>
+  <si>
+    <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/sub/v1/accounts/$BAN/subscriptions/$SUBSCRIBER/contract</t>
+  </si>
+  <si>
+    <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/sub/v1/accounts/$BAN/subscriptions/$SUBSCRIBER/upgrade-eligibility?checkEarlyUpgrade=true&amp;fetchAdditionalInfoKey=JUMPUPGRADE</t>
+  </si>
+  <si>
+    <t>upgrade-eligibility</t>
   </si>
 </sst>
 </file>
@@ -867,7 +880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -965,10 +978,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,11 +1053,33 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -1056,7 +1091,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,11 +1797,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="143.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2304,7 +2343,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,4 +2443,101 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="140.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Code modified by arjun on 12-06-2019
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INPUT_SHEET" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="143">
   <si>
     <t>2IE</t>
   </si>
@@ -452,6 +452,12 @@
   </si>
   <si>
     <t>upgrade-eligibility</t>
+  </si>
+  <si>
+    <t>current-services</t>
+  </si>
+  <si>
+    <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/v1/sub/accounts/$BAN/subscriptions/$SUBSCRIBER/current-services</t>
   </si>
 </sst>
 </file>
@@ -978,10 +984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,7 +1063,7 @@
       <c r="A6" t="s">
         <v>137</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C6" t="s">
@@ -1072,6 +1078,17 @@
         <v>139</v>
       </c>
       <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1080,9 +1097,11 @@
     <hyperlink ref="B5" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
     <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Committed by arjun on 12-09-2019
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Eclipse\eclipse-workspace\eclipse-workspace\APIAutomaiton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\Eclipse\eclipse-workspace\eclipse-workspace\APIAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340"/>
   </bookViews>
   <sheets>
     <sheet name="INPUT_SHEET" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="134">
   <si>
     <t>2IE</t>
   </si>
@@ -373,69 +373,18 @@
     <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/sub/v1/accounts/$BAN/subscriptions</t>
   </si>
   <si>
-    <t>434349902</t>
-  </si>
-  <si>
-    <t>AugUser040</t>
-  </si>
-  <si>
-    <t>4432447994</t>
-  </si>
-  <si>
-    <t>onreg-21213</t>
-  </si>
-  <si>
-    <t>ONREG-18091</t>
-  </si>
-  <si>
-    <t>ONREG-18095</t>
-  </si>
-  <si>
     <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/accounts/v1/accounts/$BAN/financial-status?realTimeInd=false&amp;isGuestPay=false</t>
   </si>
   <si>
     <t>financialstatus</t>
   </si>
   <si>
-    <t>ONREG-25212</t>
-  </si>
-  <si>
-    <t>ONREG-25329</t>
-  </si>
-  <si>
-    <t>ONREG-25213</t>
-  </si>
-  <si>
-    <t>ONREG-25783</t>
-  </si>
-  <si>
     <t>future-payments</t>
   </si>
   <si>
     <t>https://st1-apiservices-web.test.sprint.com:7441/api/process/pay/v1/accounts/$BAN/future-payments?realTimeInd=false&amp;isUsgBan=false</t>
   </si>
   <si>
-    <t>103341135</t>
-  </si>
-  <si>
-    <t>104404406</t>
-  </si>
-  <si>
-    <t>118789584</t>
-  </si>
-  <si>
-    <t>127188714</t>
-  </si>
-  <si>
-    <t>118919630</t>
-  </si>
-  <si>
-    <t>119134450</t>
-  </si>
-  <si>
-    <t>ONREG-12961</t>
-  </si>
-  <si>
     <t>https://st1-apiservices-web.test.sprint.com:7441/api/process/pay/v1/accounts/$BAN/payment-methods?isUsgBan=false&amp;isCheckAutoPayDiscount=true</t>
   </si>
   <si>
@@ -458,13 +407,37 @@
   </si>
   <si>
     <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/v1/sub/accounts/$BAN/subscriptions/$SUBSCRIBER/current-services</t>
+  </si>
+  <si>
+    <t>ONREG-19126</t>
+  </si>
+  <si>
+    <t>ONREG-19127</t>
+  </si>
+  <si>
+    <t>ONREG-17643</t>
+  </si>
+  <si>
+    <t>ONREG-17765</t>
+  </si>
+  <si>
+    <t>ONREG-19129</t>
+  </si>
+  <si>
+    <t>ONREG-19067</t>
+  </si>
+  <si>
+    <t>ONREG-19039</t>
+  </si>
+  <si>
+    <t>ONREG-18564</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,13 +480,6 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -570,7 +536,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -591,15 +557,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -884,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,75 +864,67 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>115</v>
+      <c r="A2" s="12">
+        <v>167647058</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>117</v>
+      <c r="A3" s="12">
+        <v>167651479</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12">
+        <v>169356812</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12">
+        <v>171655007</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12">
+        <v>171878073</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12">
+        <v>126237170</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12">
+        <v>126245368</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12">
+        <v>126806414</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>133</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>113526468</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -986,7 +937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1028,10 +979,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1039,10 +990,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1050,10 +1001,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1061,10 +1012,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -1072,10 +1023,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1083,10 +1034,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -2510,10 +2461,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -2521,10 +2472,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -2532,10 +2483,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -2543,10 +2494,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Code committed by arjun on 12-10-2019 by arjun
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INPUT_SHEET" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="137">
   <si>
     <t>2IE</t>
   </si>
@@ -431,6 +431,15 @@
   </si>
   <si>
     <t>ONREG-18564</t>
+  </si>
+  <si>
+    <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/eligibility/v1/flows?type=CHANGE_SERVICES&amp;subscriberId=$SUBSCRIBER&amp;accountId=$BAN&amp;accountSubscriberIds=$SUBSCRIBER&amp;role=ACCOUNT_OWNER</t>
+  </si>
+  <si>
+    <t>v1-flows</t>
+  </si>
+  <si>
+    <t>AugUser040</t>
   </si>
 </sst>
 </file>
@@ -843,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,6 +936,14 @@
         <v>133</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>434349902</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -935,7 +952,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -1040,6 +1057,17 @@
         <v>125</v>
       </c>
       <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code committed by arjun
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="139">
   <si>
     <t>2IE</t>
   </si>
@@ -409,37 +409,43 @@
     <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/v1/sub/accounts/$BAN/subscriptions/$SUBSCRIBER/current-services</t>
   </si>
   <si>
-    <t>ONREG-19126</t>
-  </si>
-  <si>
-    <t>ONREG-19127</t>
-  </si>
-  <si>
-    <t>ONREG-17643</t>
-  </si>
-  <si>
-    <t>ONREG-17765</t>
-  </si>
-  <si>
-    <t>ONREG-19129</t>
-  </si>
-  <si>
-    <t>ONREG-19067</t>
-  </si>
-  <si>
-    <t>ONREG-19039</t>
-  </si>
-  <si>
-    <t>ONREG-18564</t>
-  </si>
-  <si>
     <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/eligibility/v1/flows?type=CHANGE_SERVICES&amp;subscriberId=$SUBSCRIBER&amp;accountId=$BAN&amp;accountSubscriberIds=$SUBSCRIBER&amp;role=ACCOUNT_OWNER</t>
   </si>
   <si>
     <t>v1-flows</t>
   </si>
   <si>
-    <t>AugUser040</t>
+    <t>https://st1-apiservices-sen.test.sprint.com:8441/api/digital/mac/v1/accounts/$BAN/adjustment-codes?macInd=autopay</t>
+  </si>
+  <si>
+    <t>mac-adjustment</t>
+  </si>
+  <si>
+    <t>ONREG-17921</t>
+  </si>
+  <si>
+    <t>ONREG-13083</t>
+  </si>
+  <si>
+    <t>ONREG-17938</t>
+  </si>
+  <si>
+    <t>ONREG-13431</t>
+  </si>
+  <si>
+    <t>ONREG-17964</t>
+  </si>
+  <si>
+    <t>ONREG-17855</t>
+  </si>
+  <si>
+    <t>ONREG-17891</t>
+  </si>
+  <si>
+    <t>ONREG-19823</t>
+  </si>
+  <si>
+    <t>ONREG-13182</t>
   </si>
 </sst>
 </file>
@@ -855,7 +861,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,74 +880,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <v>167647058</v>
+        <v>100439175</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
-        <v>167651479</v>
+        <v>100567017</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
-        <v>169356812</v>
+        <v>101487374</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
-        <v>171655007</v>
+        <v>101828015</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
-        <v>171878073</v>
+        <v>103385568</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
-        <v>126237170</v>
+        <v>105805094</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
-        <v>126245368</v>
+        <v>108362572</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
-        <v>126806414</v>
+        <v>113556403</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
-        <v>434349902</v>
+        <v>136524851</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -952,10 +958,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,14 +990,11 @@
       <c r="A2" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>113</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1009,7 +1012,7 @@
       <c r="A4" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>117</v>
       </c>
       <c r="C4" t="s">
@@ -1020,7 +1023,7 @@
       <c r="A5" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>118</v>
       </c>
       <c r="C5" t="s">
@@ -1062,12 +1065,23 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2442,10 +2456,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C8"/>
+      <selection activeCell="A2" sqref="A2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2550,6 +2564,28 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>

</xml_diff>

<commit_message>
Code committed by arjun on 12/16/2019
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="136">
   <si>
     <t>2IE</t>
   </si>
@@ -430,7 +430,13 @@
     <t>ONREG-19705</t>
   </si>
   <si>
-    <t>ST1-27775</t>
+    <t>ONREG-25688</t>
+  </si>
+  <si>
+    <t>266720569</t>
+  </si>
+  <si>
+    <t>ONREG-20095</t>
   </si>
 </sst>
 </file>
@@ -843,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +861,7 @@
     <col min="2" max="2" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -863,37 +869,55 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>155283019</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>162691762</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>202592941</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
-        <v>131507015</v>
+        <v>288561502</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>133</v>
       </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code Committed by arjun 01-04-2020
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="175">
   <si>
     <t>2IE</t>
   </si>
@@ -446,15 +446,6 @@
     <t>https://st2-apiservices-sen.test.sprint.com:8442/api/digital/mac/v1/accounts/$BAN/adjustment-codes?macInd=autopay</t>
   </si>
   <si>
-    <t>TWREG-50568</t>
-  </si>
-  <si>
-    <t>TWREG-50226</t>
-  </si>
-  <si>
-    <t>TWREG-51112</t>
-  </si>
-  <si>
     <t>https://st2-apiservices-sen.test.sprint.com:8442/api/digital/v1/subscriberInfo/lookup/subscriberbasicinfo</t>
   </si>
   <si>
@@ -546,6 +537,27 @@
   </si>
   <si>
     <t>accountplans</t>
+  </si>
+  <si>
+    <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/accountplans/v1/accounts/$BAN/plans?userRole=ACCOUNT_OWNER</t>
+  </si>
+  <si>
+    <t>v1-services</t>
+  </si>
+  <si>
+    <t>https://st1-apiservices-sen.test.sprint.com:8441/api/process/products/v1/services?lineDetail=lineType=CHANGE_SERVICES;subscriberID=$SUBSCRIBER</t>
+  </si>
+  <si>
+    <t>https://st2-apiservices-sen.test.sprint.com:8442/api/process/products/v1/services?lineDetail=lineType=CHANGE_SERVICES;subscriberID=$SUBSCRIBER</t>
+  </si>
+  <si>
+    <t>ONREG-19077</t>
+  </si>
+  <si>
+    <t>ONREG-20177</t>
+  </si>
+  <si>
+    <t>ONREG-20230</t>
   </si>
 </sst>
 </file>
@@ -597,10 +609,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -678,12 +690,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -693,6 +699,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -980,7 +992,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,28 +1009,28 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>100001707</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>100108528</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>100096119</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>139</v>
+    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>127890560</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>120607864</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>149298381</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1029,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,7 +1069,7 @@
         <v>102</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1065,41 +1077,32 @@
         <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
+      <c r="D2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A3" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C3" s="12" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2464,10 +2467,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2492,7 +2495,7 @@
         <v>102</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2546,7 +2549,7 @@
       <c r="A6" t="s">
         <v>120</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>121</v>
       </c>
       <c r="C6" t="s">
@@ -2587,7 +2590,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>129</v>
       </c>
       <c r="B10" t="s">
@@ -2598,116 +2601,138 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B11" s="14" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="B12" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="E11" s="14" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="B13" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="C12" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
+      <c r="D14" s="12"/>
+      <c r="E14" s="12" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B15" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
+      <c r="D15" s="12"/>
+      <c r="E15" s="12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B16" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14" t="s">
+      <c r="C16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="B17" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="C17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="B18" s="15" t="s">
+      <c r="A18" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2716,18 +2741,21 @@
     <hyperlink ref="B5" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
     <hyperlink ref="B18" r:id="rId3"/>
+    <hyperlink ref="B19" r:id="rId4"/>
+    <hyperlink ref="B20" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2750,7 +2778,7 @@
         <v>102</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2853,116 +2881,138 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="B11" s="14" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="C12" s="14" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B13" s="14" t="s">
+      <c r="D14" s="12"/>
+      <c r="E14" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="C18" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="C18" s="14" t="s">
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2971,6 +3021,8 @@
     <hyperlink ref="B5" r:id="rId1" display="https://st1-apiservices-web.test.sprint.com:7441/api/process/pay/v1/accounts/$BAN/payment-methods?isUsgBan=false&amp;isCheckAutoPayDiscount=true"/>
     <hyperlink ref="B4" r:id="rId2" display="https://st1-apiservices-web.test.sprint.com:7441/api/process/pay/v1/accounts/$BAN/future-payments?realTimeInd=false&amp;isUsgBan=false"/>
     <hyperlink ref="B18" r:id="rId3"/>
+    <hyperlink ref="B19" r:id="rId4"/>
+    <hyperlink ref="B20" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Code committed by Arjun 01/10/2020
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13875" windowHeight="5340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INPUT_SHEET" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="196">
   <si>
     <t>2IE</t>
   </si>
@@ -560,31 +560,67 @@
     <t>https://st2-apiservices-sen.test.sprint.com:8442/api/process/products/v1/plans?lineDetail=lineType=CHANGE_PLAN;subscriberID=$SUBSCRIBER</t>
   </si>
   <si>
-    <t>TWREG-48091</t>
-  </si>
-  <si>
-    <t>TWREG-61417</t>
-  </si>
-  <si>
-    <t>ST2-62425</t>
-  </si>
-  <si>
-    <t>TWREG-46810</t>
-  </si>
-  <si>
-    <t>TWREG-61404</t>
-  </si>
-  <si>
-    <t>ST2-64571</t>
-  </si>
-  <si>
-    <t>REG-JAN-ITE2-1003</t>
-  </si>
-  <si>
-    <t>TWREG-50042</t>
-  </si>
-  <si>
-    <t>TWREG-61166</t>
+    <t>ONREG-19030</t>
+  </si>
+  <si>
+    <t>ONREG-20195</t>
+  </si>
+  <si>
+    <t>ONREG-17902</t>
+  </si>
+  <si>
+    <t>ONREG-17988</t>
+  </si>
+  <si>
+    <t>ONREG-12961</t>
+  </si>
+  <si>
+    <t>ST1-28486</t>
+  </si>
+  <si>
+    <t>ONREG-18176</t>
+  </si>
+  <si>
+    <t>ONREG-18408</t>
+  </si>
+  <si>
+    <t>ONREG-21972</t>
+  </si>
+  <si>
+    <t>ONREG-13351</t>
+  </si>
+  <si>
+    <t>ONREG-15364</t>
+  </si>
+  <si>
+    <t>ONREG-12954</t>
+  </si>
+  <si>
+    <t>ONREG-26139</t>
+  </si>
+  <si>
+    <t>ONREG-24328</t>
+  </si>
+  <si>
+    <t>ONREG-17951</t>
+  </si>
+  <si>
+    <t>ONREG-25063</t>
+  </si>
+  <si>
+    <t>ST1-29626</t>
+  </si>
+  <si>
+    <t>ONREG-25938</t>
+  </si>
+  <si>
+    <t>ONREG-13929</t>
+  </si>
+  <si>
+    <t>ST1-29643</t>
+  </si>
+  <si>
+    <t>ST1-30195</t>
   </si>
 </sst>
 </file>
@@ -721,7 +757,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
@@ -1005,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1065,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
-        <v>129835926</v>
+        <v>110909712</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>175</v>
@@ -1035,7 +1073,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16">
-        <v>110756749</v>
+        <v>101135374</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>176</v>
@@ -1043,7 +1081,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
-        <v>266707755</v>
+        <v>109069454</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>177</v>
@@ -1051,7 +1089,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
-        <v>103675616</v>
+        <v>105419461</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>178</v>
@@ -1059,7 +1097,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
-        <v>148228772</v>
+        <v>113526468</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>179</v>
@@ -1067,7 +1105,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
-        <v>382040443</v>
+        <v>114883075</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>180</v>
@@ -1075,7 +1113,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
-        <v>100336058</v>
+        <v>117878109</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>181</v>
@@ -1083,7 +1121,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
-        <v>361262845</v>
+        <v>111805815</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>182</v>
@@ -1091,10 +1129,114 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="16">
-        <v>231972919</v>
+        <v>153077753</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>131704213</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>130485588</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>174719210</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>174164117</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>191784271</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>102642966</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <v>362021567</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>109069454</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>797577467</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>145455414</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <v>716645783</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>810021262</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <v>265596532</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1108,7 +1250,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,19 +1282,22 @@
       <c r="A2" t="s">
         <v>106</v>
       </c>
-      <c r="B2" t="s">
-        <v>130</v>
+      <c r="B2" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1160,10 +1305,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1171,77 +1316,86 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
+      <c r="A6" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
+      <c r="A7" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="A8" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" t="s">
-        <v>135</v>
+        <v>167</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="A10" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://st1-apiservices-web.test.sprint.com:7441/api/process/pay/v1/accounts/$BAN/payment-methods?isUsgBan=false&amp;isCheckAutoPayDiscount=true"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://st1-apiservices-web.test.sprint.com:7441/api/process/pay/v1/accounts/$BAN/future-payments?realTimeInd=false&amp;isUsgBan=false"/>
+    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2608,8 +2762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Committed by arjun 01-12-2020
</commit_message>
<xml_diff>
--- a/APIInput.xlsx
+++ b/APIInput.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Sheet1" sheetId="4" state="hidden" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="6" state="hidden" r:id="rId5"/>
     <sheet name="Sheet2" sheetId="5" state="hidden" r:id="rId6"/>
-    <sheet name="GUIDELINES" sheetId="3" r:id="rId7"/>
+    <sheet name="Gudie Lines" sheetId="3" r:id="rId7"/>
     <sheet name="TestURLinfoST1" sheetId="8" r:id="rId8"/>
     <sheet name="TestURLinfoST2" sheetId="9" r:id="rId9"/>
   </sheets>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="280">
   <si>
     <t>2IE</t>
   </si>
@@ -167,9 +167,6 @@
     <t>3. Replacing the multiple variables in request body will be treated as enhancement</t>
   </si>
   <si>
-    <t>4. Handling Multiple endpoints is not in scope ex: fetching subscriber ids and replacing them in next call for lookup/services</t>
-  </si>
-  <si>
     <t>https://st2-apiservices-web.test.sprint.com:7441/api/process/pay/v1/v1/accounts/$BAN/payment-methods?isUsgBan=false&amp;isCheckAutoPayDiscount=false</t>
   </si>
   <si>
@@ -560,35 +557,329 @@
     <t>https://st2-apiservices-sen.test.sprint.com:8442/api/process/products/v1/plans?lineDetail=lineType=CHANGE_PLAN;subscriberID=$SUBSCRIBER</t>
   </si>
   <si>
-    <t>TWREG-51125</t>
-  </si>
-  <si>
-    <t>TWREG-51534</t>
-  </si>
-  <si>
-    <t>TWREG-55244</t>
-  </si>
-  <si>
-    <t>TWREG-55600</t>
-  </si>
-  <si>
-    <t>TWREG-59505</t>
-  </si>
-  <si>
-    <t>TWREG-50368</t>
-  </si>
-  <si>
-    <t>TWREG-56300</t>
-  </si>
-  <si>
-    <t>TWREG-56725</t>
+    <t>v1-plans-errorhandlingpending</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>querysubscriberresourcehistorylist</t>
+  </si>
+  <si>
+    <t>https://st2-apiservices-sen.test.sprint.com:8442/api/resourceinfo/1.0/querysubscriberresourcehistorylist/$SUBSCRIBER?idField=subscriberId</t>
+  </si>
+  <si>
+    <t>TWREG-52678</t>
+  </si>
+  <si>
+    <t>TWREG-49016</t>
+  </si>
+  <si>
+    <t>TWREG-47806</t>
+  </si>
+  <si>
+    <t>TWREG-52847</t>
+  </si>
+  <si>
+    <t>147266306</t>
+  </si>
+  <si>
+    <t>TWREG-49139</t>
+  </si>
+  <si>
+    <t>146796612</t>
+  </si>
+  <si>
+    <t>TWREG-52691</t>
+  </si>
+  <si>
+    <t>148040760</t>
+  </si>
+  <si>
+    <t>TWREG-47792</t>
+  </si>
+  <si>
+    <t>149065716</t>
+  </si>
+  <si>
+    <t>TWREG-52702</t>
+  </si>
+  <si>
+    <t>146935086</t>
+  </si>
+  <si>
+    <t>TWREG-48528</t>
+  </si>
+  <si>
+    <t>146038187</t>
+  </si>
+  <si>
+    <t>TWREG-48976</t>
+  </si>
+  <si>
+    <t>145440683</t>
+  </si>
+  <si>
+    <t>TWREG-47601</t>
+  </si>
+  <si>
+    <t>146662202</t>
+  </si>
+  <si>
+    <t>TWREG-49067</t>
+  </si>
+  <si>
+    <t>145542103</t>
+  </si>
+  <si>
+    <t>TWREG-49219</t>
+  </si>
+  <si>
+    <t>145620261</t>
+  </si>
+  <si>
+    <t>TWREG-49182</t>
+  </si>
+  <si>
+    <t>148954997</t>
+  </si>
+  <si>
+    <t>TWREG-48338</t>
+  </si>
+  <si>
+    <t>149239716</t>
+  </si>
+  <si>
+    <t>TWREG-52709</t>
+  </si>
+  <si>
+    <t>149333261</t>
+  </si>
+  <si>
+    <t>TWREG-52705</t>
+  </si>
+  <si>
+    <t>149581863</t>
+  </si>
+  <si>
+    <t>TWREG-49443</t>
+  </si>
+  <si>
+    <t>147960244</t>
+  </si>
+  <si>
+    <t>TWREG-47807</t>
+  </si>
+  <si>
+    <t>148028043</t>
+  </si>
+  <si>
+    <t>TWREG-47805</t>
+  </si>
+  <si>
+    <t>148352331</t>
+  </si>
+  <si>
+    <t>TWREG-47935</t>
+  </si>
+  <si>
+    <t>149406219</t>
+  </si>
+  <si>
+    <t>TWREG-48521</t>
+  </si>
+  <si>
+    <t>149559235</t>
+  </si>
+  <si>
+    <t>TWREG-51599</t>
+  </si>
+  <si>
+    <t>147566558</t>
+  </si>
+  <si>
+    <t>TWREG-52942</t>
+  </si>
+  <si>
+    <t>147744941</t>
+  </si>
+  <si>
+    <t>TWREG-49441</t>
+  </si>
+  <si>
+    <t>147849599</t>
+  </si>
+  <si>
+    <t>TWREG-47800</t>
+  </si>
+  <si>
+    <t>148044219</t>
+  </si>
+  <si>
+    <t>TWREG-51699</t>
+  </si>
+  <si>
+    <t>146811413</t>
+  </si>
+  <si>
+    <t>TWREG-48989</t>
+  </si>
+  <si>
+    <t>147274674</t>
+  </si>
+  <si>
+    <t>TWREG-48341</t>
+  </si>
+  <si>
+    <t>147314173</t>
+  </si>
+  <si>
+    <t>TWREG-52577</t>
+  </si>
+  <si>
+    <t>147117964</t>
+  </si>
+  <si>
+    <t>TWREG-47818</t>
+  </si>
+  <si>
+    <t>147815470</t>
+  </si>
+  <si>
+    <t>TWREG-48939</t>
+  </si>
+  <si>
+    <t>147378118</t>
+  </si>
+  <si>
+    <t>TWREG-49292</t>
+  </si>
+  <si>
+    <t>148141994</t>
+  </si>
+  <si>
+    <t>TWREG-47172</t>
+  </si>
+  <si>
+    <t>148331789</t>
+  </si>
+  <si>
+    <t>TWREG-47902</t>
+  </si>
+  <si>
+    <t>148545759</t>
+  </si>
+  <si>
+    <t>TWREG-52680</t>
+  </si>
+  <si>
+    <t>148753609</t>
+  </si>
+  <si>
+    <t>TWREG-49291</t>
+  </si>
+  <si>
+    <t>148800953</t>
+  </si>
+  <si>
+    <t>TWREG-52682</t>
+  </si>
+  <si>
+    <t>148841076</t>
+  </si>
+  <si>
+    <t>TWREG-52996</t>
+  </si>
+  <si>
+    <t>148123566</t>
+  </si>
+  <si>
+    <t>TWREG-47803</t>
+  </si>
+  <si>
+    <t>148941481</t>
+  </si>
+  <si>
+    <t>TWREG-47889</t>
+  </si>
+  <si>
+    <t>148217003</t>
+  </si>
+  <si>
+    <t>TWREG-52684</t>
+  </si>
+  <si>
+    <t>148860778</t>
+  </si>
+  <si>
+    <t>TWREG-49282</t>
+  </si>
+  <si>
+    <t>585116502</t>
+  </si>
+  <si>
+    <t>ST2-61683</t>
+  </si>
+  <si>
+    <t>593821019</t>
+  </si>
+  <si>
+    <t>ST2-67251</t>
+  </si>
+  <si>
+    <t>638016758</t>
+  </si>
+  <si>
+    <t>ST2-66434</t>
+  </si>
+  <si>
+    <t>605023054</t>
+  </si>
+  <si>
+    <t>ST2-67260</t>
+  </si>
+  <si>
+    <t>632990415</t>
+  </si>
+  <si>
+    <t>ST2-67277</t>
+  </si>
+  <si>
+    <t>636267990</t>
+  </si>
+  <si>
+    <t>ST2-67283</t>
+  </si>
+  <si>
+    <t>634343869</t>
+  </si>
+  <si>
+    <t>ST2-67279</t>
+  </si>
+  <si>
+    <t>563464336</t>
+  </si>
+  <si>
+    <t>ST2-66104</t>
+  </si>
+  <si>
+    <t>633417305</t>
+  </si>
+  <si>
+    <t>ST2-61701</t>
+  </si>
+  <si>
+    <t>630119400</t>
+  </si>
+  <si>
+    <t>ST2-66552</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,8 +923,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF505050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -653,6 +950,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -687,7 +990,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -718,6 +1021,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
@@ -1001,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="A10:XFD15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,71 +1328,431 @@
         <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>100037210</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>175</v>
+      <c r="A2" s="16">
+        <v>148747413</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>100134144</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>176</v>
+      <c r="A3">
+        <v>149510681</v>
+      </c>
+      <c r="B3" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>157292133</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>177</v>
+      <c r="A4">
+        <v>146745019</v>
+      </c>
+      <c r="B4" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>389117267</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>178</v>
+      <c r="A5">
+        <v>147253016</v>
+      </c>
+      <c r="B5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>130010057</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>179</v>
+      <c r="A6" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>140901976</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>180</v>
+      <c r="A7" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>145979901</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>181</v>
+      <c r="A8" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>166576293</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>182</v>
+      <c r="A9" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -1093,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD21"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,18 +1788,18 @@
         <v>17</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1137,7 +1807,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -1148,10 +1818,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1159,10 +1829,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -1170,12 +1840,203 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
         <v>133</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1183,9 +2044,13 @@
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" display="https://st1-apiservices-web.test.sprint.com:7441/api/process/pay/v1/accounts/$BAN/payment-methods?isUsgBan=false&amp;isCheckAutoPayDiscount=true"/>
     <hyperlink ref="B4" r:id="rId2" display="https://st1-apiservices-web.test.sprint.com:7441/api/process/pay/v1/accounts/$BAN/future-payments?realTimeInd=false&amp;isUsgBan=false"/>
+    <hyperlink ref="B18" r:id="rId3"/>
+    <hyperlink ref="B19" r:id="rId4"/>
+    <hyperlink ref="B20" r:id="rId5"/>
+    <hyperlink ref="B21" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1213,61 +2078,61 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" t="s">
         <v>102</v>
-      </c>
-      <c r="E1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>107</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>111</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1292,10 +2157,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -1316,15 +2181,15 @@
         <v>1000</v>
       </c>
       <c r="K1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1345,7 +2210,7 @@
         <v>1000</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1484,15 +2349,15 @@
         <v>1000</v>
       </c>
       <c r="K10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -1513,15 +2378,15 @@
         <v>1000</v>
       </c>
       <c r="K11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -1542,20 +2407,20 @@
         <v>1000</v>
       </c>
       <c r="K12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -1576,15 +2441,15 @@
         <v>1000</v>
       </c>
       <c r="K16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -1605,15 +2470,15 @@
         <v>1000</v>
       </c>
       <c r="K17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -1634,7 +2499,7 @@
         <v>1000</v>
       </c>
       <c r="K18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1663,7 +2528,7 @@
         <v>1000</v>
       </c>
       <c r="K19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1692,17 +2557,17 @@
         <v>1000</v>
       </c>
       <c r="K20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1717,152 +2582,152 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1886,7 +2751,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>GUIDELINES!#REF!</xm:f>
+            <xm:f>'Gudie Lines'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>A7:A8</xm:sqref>
         </x14:dataValidation>
@@ -1939,15 +2804,15 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>24</v>
@@ -1971,18 +2836,18 @@
         <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -2003,15 +2868,15 @@
         <v>1000</v>
       </c>
       <c r="J3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
@@ -2035,15 +2900,15 @@
         <v>1000</v>
       </c>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
@@ -2067,21 +2932,21 @@
         <v>1000</v>
       </c>
       <c r="J8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -2102,18 +2967,18 @@
         <v>1000</v>
       </c>
       <c r="J9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>24</v>
@@ -2137,13 +3002,13 @@
         <v>1000</v>
       </c>
       <c r="J10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2167,7 +3032,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>24</v>
@@ -2191,15 +3056,15 @@
         <v>1000</v>
       </c>
       <c r="J1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>24</v>
@@ -2223,15 +3088,15 @@
         <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
@@ -2255,12 +3120,12 @@
         <v>1000</v>
       </c>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>24</v>
@@ -2284,15 +3149,15 @@
         <v>1000</v>
       </c>
       <c r="J7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -2313,12 +3178,12 @@
         <v>1000</v>
       </c>
       <c r="J8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
@@ -2342,24 +3207,24 @@
         <v>1000</v>
       </c>
       <c r="J9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2369,22 +3234,22 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -2394,32 +3259,32 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -2429,7 +3294,7 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2443,10 +3308,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,21 +3404,49 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="9" t="s">
-        <v>44</v>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="14" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="B15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2575,32 +3468,32 @@
         <v>17</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -2608,10 +3501,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -2619,10 +3512,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -2630,10 +3523,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -2641,10 +3534,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -2652,10 +3545,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" t="s">
         <v>124</v>
-      </c>
-      <c r="B8" t="s">
-        <v>125</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -2663,10 +3556,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -2674,10 +3567,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -2685,87 +3578,87 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>140</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>145</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>147</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>148</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>150</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>151</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>153</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>154</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>7</v>
@@ -2775,10 +3668,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>156</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>7</v>
@@ -2788,10 +3681,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>7</v>
@@ -2799,10 +3692,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -2810,23 +3703,12 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="C20" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C21" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2846,10 +3728,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,18 +3751,18 @@
         <v>17</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -2888,7 +3770,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -2899,10 +3781,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -2910,10 +3792,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -2921,10 +3803,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -2932,10 +3814,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -2943,10 +3825,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -2954,10 +3836,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -2965,10 +3847,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -2976,87 +3858,87 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>140</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>7</v>
@@ -3066,10 +3948,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>7</v>
@@ -3079,10 +3961,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" t="s">
         <v>163</v>
-      </c>
-      <c r="B18" t="s">
-        <v>164</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>7</v>
@@ -3090,10 +3972,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -3101,23 +3983,12 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="B21" t="s">
-        <v>174</v>
-      </c>
-      <c r="C21" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3128,7 +3999,6 @@
     <hyperlink ref="B18" r:id="rId3"/>
     <hyperlink ref="B19" r:id="rId4"/>
     <hyperlink ref="B20" r:id="rId5"/>
-    <hyperlink ref="B21" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>